<commit_message>
improve logging, add disk cache
</commit_message>
<xml_diff>
--- a/reports/model_comparisons.xlsx
+++ b/reports/model_comparisons.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Model Name</t>
   </si>
@@ -38,66 +38,27 @@
     <t>Mean Confidence</t>
   </si>
   <si>
-    <t>llama3_8b-instruct-sentiment_analysis-q4_K_M</t>
-  </si>
-  <si>
-    <t>llama3_8b-instruct-sentiment_analysis-q5_K_M</t>
-  </si>
-  <si>
-    <t>llama3_8b-instruct-sentiment_analysis-q8_0</t>
-  </si>
-  <si>
     <t>llama3_8b-instruct-sentiment_analysis-fp16</t>
   </si>
   <si>
-    <t>llama3_8b-instruct-q4_K_M</t>
-  </si>
-  <si>
-    <t>llama3_8b-instruct-q5_K_M</t>
-  </si>
-  <si>
-    <t>llama3_8b-instruct-q8_0</t>
-  </si>
-  <si>
     <t>llama3_8b-instruct-fp16</t>
   </si>
   <si>
-    <t>mistral_7b-instruct-q4_K_M</t>
-  </si>
-  <si>
-    <t>mistral_7b-instruct-q5_K_M</t>
-  </si>
-  <si>
-    <t>mistral_7b-instruct-q8_0</t>
+    <t>mistral-7b-sentiment-may-18-2024-1epoch-unsloth.F16</t>
   </si>
   <si>
     <t>mistral_7b-instruct-fp16</t>
   </si>
   <si>
-    <t>dolphin-mistral_7b-v2.8-q4_K_M</t>
-  </si>
-  <si>
-    <t>dolphin-mistral_7b-v2.8-q5_K_M</t>
-  </si>
-  <si>
-    <t>dolphin-mistral_7b-v2.8-q8_0</t>
-  </si>
-  <si>
     <t>dolphin-mistral_7b-v2.8-fp16</t>
   </si>
   <si>
-    <t>q4_K_M</t>
-  </si>
-  <si>
-    <t>q5_K_M</t>
-  </si>
-  <si>
-    <t>q8_0</t>
-  </si>
-  <si>
     <t>fp16</t>
   </si>
   <si>
+    <t>unsloth.F16</t>
+  </si>
+  <si>
     <t>Comparison</t>
   </si>
   <si>
@@ -116,37 +77,16 @@
     <t>llama3_8b-instruct-fp16 vs llama3_8b-instruct-sentiment_analysis-fp16</t>
   </si>
   <si>
-    <t>llama3_8b-instruct-q4_K_M vs llama3_8b-instruct-sentiment_analysis-q4_K_M</t>
-  </si>
-  <si>
-    <t>llama3_8b-instruct-q5_K_M vs llama3_8b-instruct-sentiment_analysis-q5_K_M</t>
-  </si>
-  <si>
-    <t>llama3_8b-instruct-q8_0 vs llama3_8b-instruct-sentiment_analysis-q8_0</t>
-  </si>
-  <si>
     <t>mistral_7b-instruct-fp16 vs llama3_8b-instruct-fp16</t>
   </si>
   <si>
-    <t>mistral_7b-instruct-q4_K_M vs llama3_8b-instruct-q4_K_M</t>
-  </si>
-  <si>
-    <t>mistral_7b-instruct-q5_K_M vs llama3_8b-instruct-q5_K_M</t>
-  </si>
-  <si>
-    <t>mistral_7b-instruct-q8_0 vs llama3_8b-instruct-q8_0</t>
-  </si>
-  <si>
     <t>dolphin-mistral_7b-v2.8-fp16 vs mistral_7b-instruct-fp16</t>
   </si>
   <si>
-    <t>dolphin-mistral_7b-v2.8-q4_K_M vs mistral_7b-instruct-q4_K_M</t>
-  </si>
-  <si>
-    <t>dolphin-mistral_7b-v2.8-q5_K_M vs mistral_7b-instruct-q5_K_M</t>
-  </si>
-  <si>
-    <t>dolphin-mistral_7b-v2.8-q8_0 vs mistral_7b-instruct-q8_0</t>
+    <t>mistral-7b-sentiment-may-18-2024-1epoch-unsloth.F16 vs mistral_7b-instruct-fp16</t>
+  </si>
+  <si>
+    <t>mistral-7b-sentiment-may-18-2024-1epoch-unsloth.F16 vs llama3_8b-instruct-sentiment_analysis-fp16</t>
   </si>
 </sst>
 </file>
@@ -504,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -538,22 +478,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>3.485</v>
+        <v>7.841</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
       <c r="F2">
-        <v>0.501</v>
+        <v>0.356</v>
       </c>
       <c r="G2">
-        <v>0.8129999999999999</v>
+        <v>0.768</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -561,22 +501,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>4.158</v>
+        <v>7.839</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0.116</v>
+        <v>0.176</v>
       </c>
       <c r="F3">
-        <v>0.595</v>
+        <v>0.364</v>
       </c>
       <c r="G3">
-        <v>0.856</v>
+        <v>0.852</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -584,22 +524,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C4">
-        <v>4.847</v>
+        <v>8.464</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.125</v>
+        <v>0.13</v>
       </c>
       <c r="F4">
-        <v>0.534</v>
+        <v>0.482</v>
       </c>
       <c r="G4">
-        <v>0.832</v>
+        <v>0.772</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -607,22 +547,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>7.952</v>
+        <v>8.858000000000001</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0.764</v>
       </c>
       <c r="E5">
-        <v>0.141</v>
+        <v>0.093</v>
       </c>
       <c r="F5">
-        <v>0.535</v>
+        <v>0.455</v>
       </c>
       <c r="G5">
-        <v>0.837</v>
+        <v>0.853</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -630,275 +570,22 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>3.537</v>
+        <v>8.718999999999999</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0.298</v>
+        <v>0.098</v>
       </c>
       <c r="F6">
-        <v>0.361</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="G6">
-        <v>0.866</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7">
-        <v>4.281</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>0.36</v>
-      </c>
-      <c r="F7">
-        <v>0.311</v>
-      </c>
-      <c r="G7">
-        <v>0.867</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8">
-        <v>4.936</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>0.309</v>
-      </c>
-      <c r="F8">
-        <v>0.371</v>
-      </c>
-      <c r="G8">
-        <v>0.867</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9">
-        <v>7.936</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>0.302</v>
-      </c>
-      <c r="F9">
-        <v>0.354</v>
-      </c>
-      <c r="G9">
-        <v>0.876</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10">
-        <v>4.07</v>
-      </c>
-      <c r="D10">
-        <v>0.6879999999999999</v>
-      </c>
-      <c r="E10">
-        <v>0.138</v>
-      </c>
-      <c r="F10">
-        <v>0.405</v>
-      </c>
-      <c r="G10">
-        <v>0.881</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11">
-        <v>4.578</v>
-      </c>
-      <c r="D11">
-        <v>0.768</v>
-      </c>
-      <c r="E11">
-        <v>0.113</v>
-      </c>
-      <c r="F11">
-        <v>0.463</v>
-      </c>
-      <c r="G11">
-        <v>0.859</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12">
-        <v>5.159</v>
-      </c>
-      <c r="D12">
-        <v>0.741</v>
-      </c>
-      <c r="E12">
-        <v>0.134</v>
-      </c>
-      <c r="F12">
-        <v>0.43</v>
-      </c>
-      <c r="G12">
-        <v>0.864</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13">
-        <v>8.467000000000001</v>
-      </c>
-      <c r="D13">
-        <v>0.696</v>
-      </c>
-      <c r="E13">
-        <v>0.155</v>
-      </c>
-      <c r="F13">
-        <v>0.445</v>
-      </c>
-      <c r="G13">
-        <v>0.871</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14">
-        <v>3.827</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>0.1</v>
-      </c>
-      <c r="F14">
-        <v>0.605</v>
-      </c>
-      <c r="G14">
-        <v>0.867</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15">
-        <v>5.009</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>0.248</v>
-      </c>
-      <c r="F15">
-        <v>0.365</v>
-      </c>
-      <c r="G15">
-        <v>0.836</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16">
-        <v>5.441</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>0.226</v>
-      </c>
-      <c r="F16">
-        <v>0.394</v>
-      </c>
-      <c r="G16">
-        <v>0.845</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17">
-        <v>8.872</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>0.195</v>
-      </c>
-      <c r="F17">
-        <v>0.45</v>
-      </c>
-      <c r="G17">
-        <v>0.85</v>
+        <v>0.853</v>
       </c>
     </row>
   </sheetData>
@@ -908,7 +595,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -916,67 +603,67 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B2">
-        <v>8.234999999999999</v>
+        <v>0.047</v>
       </c>
       <c r="C2">
-        <v>0.005</v>
+        <v>0.829</v>
       </c>
       <c r="D2">
-        <v>-2.87</v>
+        <v>0.216</v>
       </c>
       <c r="E2">
-        <v>0.005</v>
+        <v>0.829</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B3">
-        <v>5.184</v>
+        <v>7.12</v>
       </c>
       <c r="C3">
-        <v>0.024</v>
+        <v>0.008</v>
       </c>
       <c r="D3">
-        <v>-2.277</v>
+        <v>2.668</v>
       </c>
       <c r="E3">
-        <v>0.024</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B4">
-        <v>18.747</v>
+        <v>14.247</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>-4.33</v>
+        <v>3.775</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -984,155 +671,36 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B5">
-        <v>6.821</v>
+        <v>0.796</v>
       </c>
       <c r="C5">
-        <v>0.01</v>
+        <v>0.373</v>
       </c>
       <c r="D5">
-        <v>-2.612</v>
+        <v>0.892</v>
       </c>
       <c r="E5">
-        <v>0.01</v>
+        <v>0.373</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B6">
-        <v>1.558</v>
+        <v>13.072</v>
       </c>
       <c r="C6">
-        <v>0.214</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>1.248</v>
+        <v>3.616</v>
       </c>
       <c r="E6">
-        <v>0.214</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7">
-        <v>0.372</v>
-      </c>
-      <c r="C7">
-        <v>0.542</v>
-      </c>
-      <c r="D7">
-        <v>0.61</v>
-      </c>
-      <c r="E7">
-        <v>0.542</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8">
-        <v>4.425</v>
-      </c>
-      <c r="C8">
-        <v>0.037</v>
-      </c>
-      <c r="D8">
-        <v>2.104</v>
-      </c>
-      <c r="E8">
-        <v>0.037</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9">
-        <v>0.712</v>
-      </c>
-      <c r="C9">
-        <v>0.4</v>
-      </c>
-      <c r="D9">
-        <v>0.844</v>
-      </c>
-      <c r="E9">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10">
-        <v>0.007</v>
-      </c>
-      <c r="C10">
-        <v>0.9350000000000001</v>
-      </c>
-      <c r="D10">
-        <v>0.081</v>
-      </c>
-      <c r="E10">
-        <v>0.9350000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11">
-        <v>15.542</v>
-      </c>
-      <c r="C11">
         <v>0</v>
-      </c>
-      <c r="D11">
-        <v>3.942</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12">
-        <v>2.458</v>
-      </c>
-      <c r="C12">
-        <v>0.119</v>
-      </c>
-      <c r="D12">
-        <v>-1.568</v>
-      </c>
-      <c r="E12">
-        <v>0.119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13">
-        <v>0.338</v>
-      </c>
-      <c r="C13">
-        <v>0.5620000000000001</v>
-      </c>
-      <c r="D13">
-        <v>-0.581</v>
-      </c>
-      <c r="E13">
-        <v>0.5620000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>